<commit_message>
DWH-11: Partitioning with lost rows
</commit_message>
<xml_diff>
--- a/common/src/test/resources/spends3.xlsx
+++ b/common/src/test/resources/spends3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="93">
   <si>
     <t xml:space="preserve">S. No.</t>
   </si>
@@ -531,10 +531,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO1051"/>
+  <dimension ref="A1:AO1052"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1129" activeCellId="0" sqref="F1129"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3878,12 +3878,63 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="6"/>
-      <c r="AK51" s="7"/>
+      <c r="A51" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K51" s="4" t="n">
+        <v>77001</v>
+      </c>
+      <c r="M51" s="5" t="n">
+        <v>43136</v>
+      </c>
+      <c r="N51" s="5" t="n">
+        <v>43139</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="P51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V51" s="0" t="n">
+        <v>10.18</v>
+      </c>
+      <c r="AK51" s="7" t="n">
+        <v>797</v>
+      </c>
+      <c r="AL51" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G52" s="4"/>

</xml_diff>